<commit_message>
feat: Add declaration tutorials
</commit_message>
<xml_diff>
--- a/src/Assets/templates/Modelo_Alunos.xlsx
+++ b/src/Assets/templates/Modelo_Alunos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28209"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF6A07AC-1172-4C65-B88A-4773E45AE9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{531108F0-141F-4F86-B972-139281FB1685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1031,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:Z1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -39148,7 +39148,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="R1:Z1048576" name="Range2"/>
+    <protectedRange sqref="A1:Q1048576" name="Range1"/>
   </protectedRanges>
   <conditionalFormatting sqref="N2:Q1001">
     <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">

</xml_diff>